<commit_message>
Dec3 commit - hopefully fixed onedrive duplicates
</commit_message>
<xml_diff>
--- a/data/janelia/oconnor_trialinfo.xlsx
+++ b/data/janelia/oconnor_trialinfo.xlsx
@@ -592,9 +592,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0A7641CB02EBD45AFE4F37CA692EF9D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79e9cb911a73eacf59b9da573dc6f056">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5fbe2e07-e2b2-437b-ad34-905bae2923b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b311b4483d4b4288a25c504c05092a9" ns2:_="">
-    <xsd:import namespace="5fbe2e07-e2b2-437b-ad34-905bae2923b7"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010036A2ED3FCD64534B9F36D98846FDC9CE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="90fd2a83f5dd24583a6e3fa486adde0e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="31f590fd-802d-4981-b551-2491b26a790e" xmlns:ns3="51e3fa90-0bd2-4e45-b4ed-6252fa1132a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ff499960b4ab855a970681993178e9c" ns2:_="" ns3:_="">
+    <xsd:import namespace="31f590fd-802d-4981-b551-2491b26a790e"/>
+    <xsd:import namespace="51e3fa90-0bd2-4e45-b4ed-6252fa1132a8"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -603,14 +604,15 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
@@ -619,7 +621,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5fbe2e07-e2b2-437b-ad34-905bae2923b7" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="31f590fd-802d-4981-b551-2491b26a790e" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -632,49 +634,74 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="10" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
     <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="51e3fa90-0bd2-4e45-b4ed-6252fa1132a8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -792,12 +819,14 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="31f590fd-802d-4981-b551-2491b26a790e" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0F2050F-C49C-4E6F-B488-30BE208490F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C9C1C34-48D0-4027-BF8D-9168166521FF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>